<commit_message>
Update to effort document
</commit_message>
<xml_diff>
--- a/documentation/budget/effort_commitment.xlsx
+++ b/documentation/budget/effort_commitment.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\Phishing-Email-Button\documentation\budget\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maddi\Documents\Year 2\Professional Development\Phishing-Email-Button\documentation\budget\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3F8AED-69E1-4215-AC81-01B5E95D5D49}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{007ABC16-95E7-4F34-B4BB-E66B4AC72569}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{38A891E2-6AF6-49EC-89C7-71415C5CC21F}"/>
   </bookViews>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -229,7 +230,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -315,15 +316,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thick">
-        <color theme="9"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thick">
         <color theme="9"/>
       </left>
@@ -358,7 +350,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
@@ -417,14 +409,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="88">
+  <dxfs count="44">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -787,471 +776,31 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C0006"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1617,16 +1166,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9A4048D-0B48-4A1A-A71C-86F5C3BC7E01}">
   <dimension ref="B1:AG47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B15" workbookViewId="0">
-      <selection activeCell="G32" sqref="G32"/>
+    <sheetView tabSelected="1" topLeftCell="S12" workbookViewId="0">
+      <selection activeCell="Z25" sqref="Z25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="12" style="2"/>
-    <col min="2" max="2" width="23.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="31.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="23.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.90625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="31.54296875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="23.90625" style="2" customWidth="1"/>
     <col min="5" max="20" width="12" style="2"/>
     <col min="21" max="21" width="13" style="2" bestFit="1" customWidth="1"/>
     <col min="22" max="28" width="12" style="2"/>
@@ -1634,12 +1183,12 @@
     <col min="33" max="16384" width="12" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:33" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:33" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1650,7 +1199,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:33" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1661,7 +1210,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:33" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:33" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
@@ -1672,7 +1221,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="2:33" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:33" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="B5" s="1" t="s">
         <v>5</v>
       </c>
@@ -1683,7 +1232,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:33" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
@@ -1694,10 +1243,10 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:33" x14ac:dyDescent="0.35">
       <c r="C7" s="5"/>
     </row>
-    <row r="8" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:33" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
@@ -1715,7 +1264,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:33" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
@@ -1738,7 +1287,7 @@
       </c>
       <c r="AG9" s="1"/>
     </row>
-    <row r="10" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:33" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B10" s="1" t="s">
         <v>16</v>
       </c>
@@ -1765,7 +1314,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="2:33" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:33" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B11" s="1" t="s">
         <v>20</v>
       </c>
@@ -1789,12 +1338,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="2:33" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:33" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="I12" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:33" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C14" s="1" t="s">
         <v>27</v>
       </c>
@@ -1808,7 +1357,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="2:33" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:33" x14ac:dyDescent="0.35">
       <c r="D15" s="2">
         <v>2018</v>
       </c>
@@ -1823,7 +1372,7 @@
         <v>43396</v>
       </c>
     </row>
-    <row r="17" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:33" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E17" s="8" t="s">
         <v>28</v>
       </c>
@@ -1838,7 +1387,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="18" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:33" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E18" s="10" t="s">
         <v>15</v>
       </c>
@@ -1882,7 +1431,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="19" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:33" ht="15.5" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>45</v>
       </c>
@@ -1890,7 +1439,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:33" ht="15.5" x14ac:dyDescent="0.35">
       <c r="E20" s="2" t="s">
         <v>14</v>
       </c>
@@ -1961,7 +1510,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:33" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C21" s="1" t="s">
         <v>31</v>
       </c>
@@ -2035,7 +1584,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="2:33" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:33" s="3" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C22" s="16"/>
       <c r="D22" s="16" t="s">
         <v>32</v>
@@ -2085,7 +1634,7 @@
         <v>10.75</v>
       </c>
     </row>
-    <row r="23" spans="2:33" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:33" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="D23" s="1" t="s">
         <v>33</v>
       </c>
@@ -2193,12 +1742,12 @@
         <v>34</v>
       </c>
     </row>
-    <row r="24" spans="2:33" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C24" s="1" t="s">
         <v>41</v>
       </c>
       <c r="E24" s="23" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F24" s="24" t="s">
         <v>12</v>
@@ -2207,80 +1756,80 @@
         <v>12</v>
       </c>
       <c r="H24" s="24" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="I24" s="24" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="J24" s="24" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="K24" s="24" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L24" s="24" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M24" s="24" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="N24" s="24" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="O24" s="24" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P24" s="24" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="Q24" s="24" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R24" s="24" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="S24" s="24" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="T24" s="24" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="U24" s="24" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="V24" s="24" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="W24" s="24" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="X24" s="24" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="Y24" s="24" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="Z24" s="25" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="AC24" s="3">
-        <f t="shared" ref="AC24:AC33" si="2">COUNTIFS($E24:$AB24,$I$9) * $F$9</f>
-        <v>15.262500000000001</v>
+        <f t="shared" ref="AC24:AC29" si="2">COUNTIFS($E24:$AB24,$I$9) * $F$9</f>
+        <v>35.612500000000004</v>
       </c>
       <c r="AD24" s="3">
-        <f t="shared" ref="AD24:AD33" si="3">COUNTIFS($E24:$AB24,$I$10) * $F$10</f>
-        <v>0</v>
+        <f t="shared" ref="AD24:AD29" si="3">COUNTIFS($E24:$AB24,$I$10) * $F$10</f>
+        <v>70.612499999999997</v>
       </c>
       <c r="AE24" s="3">
-        <f t="shared" ref="AE24:AE33" si="4">COUNTIFS($E24:$AB24,$I$11) * $F$11</f>
-        <v>0</v>
+        <f t="shared" ref="AE24:AE29" si="4">COUNTIFS($E24:$AB24,$I$11) * $F$11</f>
+        <v>105.6125</v>
       </c>
       <c r="AF24" s="3">
-        <f t="shared" ref="AF24:AF33" si="5">SUM(AC24:AE24)</f>
-        <v>15.262500000000001</v>
-      </c>
-    </row>
-    <row r="25" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+        <f t="shared" ref="AF24:AF29" si="5">SUM(AC24:AE24)</f>
+        <v>211.83749999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="2:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C25" s="1" t="s">
         <v>42</v>
       </c>
@@ -2291,88 +1840,88 @@
         <v>23</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="H25" s="17" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="J25" s="17" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="K25" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L25" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M25" s="17" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="N25" s="17" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="O25" s="17" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P25" s="17" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="Q25" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R25" s="17" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="S25" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="T25" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="U25" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="V25" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="W25" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="X25" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y25" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z25" s="27" t="s">
-        <v>23</v>
+        <v>16</v>
+      </c>
+      <c r="U25" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="V25" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="W25" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="X25" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y25" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z25" s="25" t="s">
+        <v>20</v>
       </c>
       <c r="AC25" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>30.525000000000002</v>
       </c>
       <c r="AD25" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>70.612499999999997</v>
       </c>
       <c r="AE25" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>105.6125</v>
       </c>
       <c r="AF25" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+        <v>206.75</v>
+      </c>
+    </row>
+    <row r="26" spans="2:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C26" s="1" t="s">
         <v>43</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="F26" s="17" t="s">
         <v>12</v>
@@ -2381,80 +1930,80 @@
         <v>23</v>
       </c>
       <c r="H26" s="17" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="I26" s="17" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="J26" s="17" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="K26" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L26" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M26" s="17" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="N26" s="17" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="O26" s="17" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P26" s="17" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="Q26" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R26" s="17" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="S26" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="T26" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="U26" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="V26" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="W26" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="X26" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y26" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z26" s="27" t="s">
-        <v>23</v>
+        <v>16</v>
+      </c>
+      <c r="U26" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="V26" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="W26" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="X26" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y26" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z26" s="25" t="s">
+        <v>20</v>
       </c>
       <c r="AC26" s="3">
         <f t="shared" si="2"/>
-        <v>10.175000000000001</v>
+        <v>30.525000000000002</v>
       </c>
       <c r="AD26" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>70.612499999999997</v>
       </c>
       <c r="AE26" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>105.6125</v>
       </c>
       <c r="AF26" s="3">
         <f t="shared" si="5"/>
-        <v>10.175000000000001</v>
-      </c>
-    </row>
-    <row r="27" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+        <v>206.75</v>
+      </c>
+    </row>
+    <row r="27" spans="2:33" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C27" s="1" t="s">
         <v>44</v>
       </c>
@@ -2462,86 +2011,86 @@
         <v>23</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="G27" s="17" t="s">
         <v>23</v>
       </c>
       <c r="H27" s="17" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="I27" s="17" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="J27" s="17" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="K27" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L27" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M27" s="17" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="N27" s="17" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="O27" s="17" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P27" s="17" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="Q27" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R27" s="17" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="S27" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="T27" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="U27" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="V27" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="W27" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="X27" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y27" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z27" s="27" t="s">
-        <v>23</v>
+        <v>16</v>
+      </c>
+      <c r="U27" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="V27" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="W27" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="X27" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y27" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z27" s="25" t="s">
+        <v>20</v>
       </c>
       <c r="AC27" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>30.525000000000002</v>
       </c>
       <c r="AD27" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>70.612499999999997</v>
       </c>
       <c r="AE27" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>105.6125</v>
       </c>
       <c r="AF27" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+        <v>206.75</v>
+      </c>
+    </row>
+    <row r="28" spans="2:33" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C28" s="1" t="s">
         <v>35</v>
       </c>
@@ -2549,153 +2098,153 @@
         <v>23</v>
       </c>
       <c r="F28" s="17" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="G28" s="17" t="s">
         <v>23</v>
       </c>
       <c r="H28" s="17" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="I28" s="17" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="J28" s="17" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="K28" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="L28" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="M28" s="17" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="N28" s="17" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="O28" s="17" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="P28" s="17" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
       <c r="Q28" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="R28" s="17" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="S28" s="17" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="T28" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="U28" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="V28" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="W28" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="X28" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y28" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z28" s="27" t="s">
-        <v>23</v>
+        <v>16</v>
+      </c>
+      <c r="U28" s="24" t="s">
+        <v>12</v>
+      </c>
+      <c r="V28" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="W28" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="X28" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y28" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z28" s="25" t="s">
+        <v>20</v>
       </c>
       <c r="AC28" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>30.525000000000002</v>
       </c>
       <c r="AD28" s="3">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>70.612499999999997</v>
       </c>
       <c r="AE28" s="3">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>105.6125</v>
       </c>
       <c r="AF28" s="3">
         <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="2:33" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+        <v>206.75</v>
+      </c>
+    </row>
+    <row r="29" spans="2:33" ht="16" thickBot="1" x14ac:dyDescent="0.4">
       <c r="C29" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E29" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="F29" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="G29" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H29" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="I29" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="J29" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="K29" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="L29" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="M29" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="N29" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="O29" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="P29" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q29" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="R29" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="S29" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="T29" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="U29" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="V29" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="W29" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="X29" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="Y29" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="Z29" s="30" t="s">
+      <c r="E29" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="F29" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="G29" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="H29" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="I29" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="J29" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="K29" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="L29" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="M29" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="N29" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="O29" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="P29" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Q29" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="R29" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="S29" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="T29" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="U29" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="V29" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="W29" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="X29" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y29" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z29" s="29" t="s">
         <v>23</v>
       </c>
       <c r="AC29" s="3">
@@ -2715,7 +2264,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:33" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:33" ht="16" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C30" s="1"/>
       <c r="D30" s="21"/>
       <c r="E30" s="17"/>
@@ -2748,7 +2297,7 @@
       <c r="AF30" s="22"/>
       <c r="AG30" s="21"/>
     </row>
-    <row r="31" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:33" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C31" s="1"/>
       <c r="D31" s="21"/>
       <c r="E31" s="17"/>
@@ -2781,7 +2330,7 @@
       <c r="AF31" s="22"/>
       <c r="AG31" s="21"/>
     </row>
-    <row r="32" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:33" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C32" s="1"/>
       <c r="D32" s="21"/>
       <c r="E32" s="17"/>
@@ -2814,7 +2363,7 @@
       <c r="AF32" s="22"/>
       <c r="AG32" s="21"/>
     </row>
-    <row r="33" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:33" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C33" s="1"/>
       <c r="D33" s="21"/>
       <c r="E33" s="17"/>
@@ -2847,10 +2396,10 @@
       <c r="AF33" s="22"/>
       <c r="AG33" s="21"/>
     </row>
-    <row r="34" spans="2:33" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:33" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="2:33" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:33" s="3" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C35" s="16" t="s">
         <v>4</v>
       </c>
@@ -2925,7 +2474,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="36" spans="2:33" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:33" s="3" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C36" s="16"/>
       <c r="D36" s="16" t="str">
         <f>$I10</f>
@@ -3002,25 +2551,25 @@
       </c>
       <c r="AC36" s="16">
         <f>SUM(AC24:AC34)</f>
-        <v>25.4375</v>
+        <v>157.71250000000001</v>
       </c>
       <c r="AD36" s="16">
         <f>SUM(AD24:AD34)</f>
-        <v>0</v>
+        <v>353.0625</v>
       </c>
       <c r="AE36" s="16">
         <f>SUM(AE24:AE34)</f>
-        <v>0</v>
+        <v>528.0625</v>
       </c>
       <c r="AF36" s="16">
         <f>SUM(AF24:AF34)</f>
-        <v>25.4375</v>
+        <v>1038.8375000000001</v>
       </c>
       <c r="AG36" s="16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="2:33" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:33" s="3" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C37" s="16"/>
       <c r="D37" s="16" t="str">
         <f>$I11</f>
@@ -3093,23 +2642,23 @@
         <v>35</v>
       </c>
     </row>
-    <row r="38" spans="2:33" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:33" s="3" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C38" s="16"/>
       <c r="D38" s="16"/>
     </row>
-    <row r="39" spans="2:33" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:33" s="3" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C39" s="16"/>
       <c r="D39" s="16"/>
     </row>
-    <row r="40" spans="2:33" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:33" s="3" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C40" s="16"/>
       <c r="D40" s="16"/>
     </row>
-    <row r="41" spans="2:33" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:33" s="3" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C41" s="16"/>
       <c r="D41" s="16"/>
     </row>
-    <row r="42" spans="2:33" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:33" s="3" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C42" s="16" t="s">
         <v>37</v>
       </c>
@@ -3218,7 +2767,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="2:33" s="3" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:33" s="3" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="C43" s="16" t="s">
         <v>37</v>
       </c>
@@ -3282,7 +2831,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="2:33" s="3" customFormat="1" ht="46.2" x14ac:dyDescent="0.85">
+    <row r="47" spans="2:33" s="3" customFormat="1" ht="46" x14ac:dyDescent="1">
       <c r="B47" s="18" t="s">
         <v>38</v>
       </c>
@@ -3295,208 +2844,208 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="E28:Z33 E24:O27">
-    <cfRule type="cellIs" dxfId="87" priority="1" operator="between">
+  <conditionalFormatting sqref="E30:Z33 E24:O27 E28:Q29 S29:Z29 S28:T28">
+    <cfRule type="cellIs" dxfId="43" priority="1" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="42" priority="2" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="3" operator="between">
+    <cfRule type="cellIs" dxfId="41" priority="3" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF34:AF35 A32:B32 D32 AA32:XFD32">
-    <cfRule type="cellIs" dxfId="43" priority="42" operator="between">
+    <cfRule type="cellIs" dxfId="40" priority="42" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="43" operator="between">
+    <cfRule type="cellIs" dxfId="39" priority="43" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="44" operator="between">
+    <cfRule type="cellIs" dxfId="38" priority="44" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20:XFD20">
-    <cfRule type="cellIs" dxfId="40" priority="40" operator="between">
+    <cfRule type="cellIs" dxfId="37" priority="40" operator="between">
       <formula>$K$10</formula>
       <formula>$K$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="41" operator="between">
+    <cfRule type="cellIs" dxfId="36" priority="41" operator="between">
       <formula>$K$9</formula>
       <formula>$K$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35:Z37">
-    <cfRule type="cellIs" dxfId="38" priority="37" operator="between">
+    <cfRule type="cellIs" dxfId="35" priority="37" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="38" operator="between">
+    <cfRule type="cellIs" dxfId="34" priority="38" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="39" operator="between">
+    <cfRule type="cellIs" dxfId="33" priority="39" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24:D24 C25:C32 AA24:XFD24">
-    <cfRule type="cellIs" dxfId="35" priority="34" operator="between">
+    <cfRule type="cellIs" dxfId="32" priority="34" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="35" operator="between">
+    <cfRule type="cellIs" dxfId="31" priority="35" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="36" operator="between">
+    <cfRule type="cellIs" dxfId="30" priority="36" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A25:B25 D25 AA25:XFD25">
-    <cfRule type="cellIs" dxfId="32" priority="31" operator="between">
+    <cfRule type="cellIs" dxfId="29" priority="31" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="32" operator="between">
+    <cfRule type="cellIs" dxfId="28" priority="32" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="33" operator="between">
+    <cfRule type="cellIs" dxfId="27" priority="33" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A26:B26 D26 AA26:XFD26">
-    <cfRule type="cellIs" dxfId="29" priority="28" operator="between">
+    <cfRule type="cellIs" dxfId="26" priority="28" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="29" operator="between">
+    <cfRule type="cellIs" dxfId="25" priority="29" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="30" operator="between">
+    <cfRule type="cellIs" dxfId="24" priority="30" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A31:B31 D31 AA31:XFD31">
-    <cfRule type="cellIs" dxfId="26" priority="13" operator="between">
+    <cfRule type="cellIs" dxfId="23" priority="13" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="14" operator="between">
+    <cfRule type="cellIs" dxfId="22" priority="14" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="15" operator="between">
+    <cfRule type="cellIs" dxfId="21" priority="15" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A27:B27 D27 AA27:XFD27">
-    <cfRule type="cellIs" dxfId="23" priority="25" operator="between">
+    <cfRule type="cellIs" dxfId="20" priority="25" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="26" operator="between">
+    <cfRule type="cellIs" dxfId="19" priority="26" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="27" operator="between">
+    <cfRule type="cellIs" dxfId="18" priority="27" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A28:B28 D28 AA28:XFD28">
-    <cfRule type="cellIs" dxfId="20" priority="22" operator="between">
+    <cfRule type="cellIs" dxfId="17" priority="22" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="23" operator="between">
+    <cfRule type="cellIs" dxfId="16" priority="23" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="24" operator="between">
+    <cfRule type="cellIs" dxfId="15" priority="24" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A29:B29 D29 AA29:XFD29">
-    <cfRule type="cellIs" dxfId="17" priority="19" operator="between">
+    <cfRule type="cellIs" dxfId="14" priority="19" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="20" operator="between">
+    <cfRule type="cellIs" dxfId="13" priority="20" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="21" operator="between">
+    <cfRule type="cellIs" dxfId="12" priority="21" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A30:B30 D30 AA30:XFD30">
-    <cfRule type="cellIs" dxfId="14" priority="16" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="16" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="17" operator="between">
+    <cfRule type="cellIs" dxfId="10" priority="17" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="18" operator="between">
+    <cfRule type="cellIs" dxfId="9" priority="18" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A33:B33 D33 AA33:XFD33">
-    <cfRule type="cellIs" dxfId="11" priority="10" operator="between">
+    <cfRule type="cellIs" dxfId="8" priority="10" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="between">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C33">
-    <cfRule type="cellIs" dxfId="8" priority="7" operator="between">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="between">
+    <cfRule type="cellIs" dxfId="4" priority="8" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="9" operator="between">
+    <cfRule type="cellIs" dxfId="3" priority="9" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P24:Z27">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="between">
+  <conditionalFormatting sqref="P24:Z24 P26:Q27 S26:T27 R26:R29 P25:T25 U25:Z28">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="between">
       <formula>$I$11</formula>
       <formula>$I$11</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="between">
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="between">
       <formula>$I$10</formula>
       <formula>$I$10</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="between">
+    <cfRule type="cellIs" dxfId="0" priority="6" operator="between">
       <formula>$I$9</formula>
       <formula>$I$9</formula>
     </cfRule>

</xml_diff>